<commit_message>
Update Clean_Data and CodeBook
1.Update Clean_Data
2.Update Codebook
3.Update json(Experiment)
</commit_message>
<xml_diff>
--- a/1_Data/Haciahmet_2023_Psy/CodeBook_Haciahmet_2023_Psy_Exp1_Clean.xlsx
+++ b/1_Data/Haciahmet_2023_Psy/CodeBook_Haciahmet_2023_Psy_Exp1_Clean.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="10480"/>
+    <workbookView windowWidth="24750" windowHeight="10480"/>
   </bookViews>
   <sheets>
-    <sheet name="Codebook_SALT_exp1_var_Info" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>Variable_name</t>
   </si>
@@ -44,49 +44,43 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>Subject ID</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Numeric</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Participant's age in years</t>
+    <t>Participant number</t>
+  </si>
+  <si>
+    <t>Number</t>
   </si>
   <si>
     <t>Numerical</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Participant's gender</t>
-  </si>
-  <si>
-    <t>Fraw(Female);Mann(Male)</t>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Block number in the experiment; each block may contain practice or experimental trials</t>
+  </si>
+  <si>
+    <t>Trial</t>
+  </si>
+  <si>
+    <t>Trial number within the block</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Phase of the experiment for practice or formal experimental trials</t>
+  </si>
+  <si>
+    <t>TrainList1;ExpList</t>
   </si>
   <si>
     <t>Categorical</t>
   </si>
   <si>
-    <t>Handedness</t>
-  </si>
-  <si>
-    <t>Participant's dominant hand</t>
-  </si>
-  <si>
-    <t>links(Left);rechts(Right)</t>
-  </si>
-  <si>
     <t>Shape</t>
   </si>
   <si>
-    <t>Shape of the object or stimulus</t>
+    <t>Visual shape stimulus presented in the trial</t>
   </si>
   <si>
     <t>circle.png;triangle.png</t>
@@ -95,55 +89,85 @@
     <t>Label</t>
   </si>
   <si>
-    <t>Label or category assigned to the shape</t>
-  </si>
-  <si>
-    <t>Ich(Self);Fremder(Stranger)</t>
+    <t>Text label presented for matching with the shape</t>
+  </si>
+  <si>
+    <t>Ich;Fremder</t>
   </si>
   <si>
     <t>Matching</t>
   </si>
   <si>
-    <t>Type of matching task performed</t>
-  </si>
-  <si>
-    <t>Matching;Nomatching</t>
-  </si>
-  <si>
-    <t>Identity</t>
-  </si>
-  <si>
-    <t>Type of identity task performed</t>
+    <t>Type of matching task for the trial; indicates whether the shape and label match or not</t>
+  </si>
+  <si>
+    <t>Matching;Nonmatching</t>
+  </si>
+  <si>
+    <t>Label_Origin_Identity</t>
+  </si>
+  <si>
+    <t>Original identity associated with the label</t>
+  </si>
+  <si>
+    <t>Label_English_Identity</t>
+  </si>
+  <si>
+    <t>English translation of the label's identity</t>
   </si>
   <si>
     <t>Self;Stranger</t>
   </si>
   <si>
+    <t>Label_Standardized_Identity</t>
+  </si>
+  <si>
+    <t>Standardized identity for the label used across experiments</t>
+  </si>
+  <si>
+    <t>Shape_Origin_Identity</t>
+  </si>
+  <si>
+    <t>Original identity associated with the shape stimulus</t>
+  </si>
+  <si>
+    <t>Shape_English_Identity</t>
+  </si>
+  <si>
+    <t>English translation of the shape's identity</t>
+  </si>
+  <si>
+    <t>Shape_Standardized_Identity</t>
+  </si>
+  <si>
+    <t>Standardized identity for the shape used across experiments</t>
+  </si>
+  <si>
     <t>Response</t>
   </si>
   <si>
-    <t>Participant's response to the task</t>
-  </si>
-  <si>
-    <t>1;5</t>
+    <t>Participant's response in the trial</t>
+  </si>
+  <si>
+    <t>1.0;5.0</t>
   </si>
   <si>
     <t>RT_ms</t>
   </si>
   <si>
-    <t>Reaction time in milliseconds</t>
+    <t>Reaction time for the response, measured in milliseconds</t>
   </si>
   <si>
     <t>RT_sec</t>
   </si>
   <si>
-    <t>Reaction time in seconds</t>
+    <t>Reaction time for the response, measured in seconds</t>
   </si>
   <si>
     <t>ACC</t>
   </si>
   <si>
-    <t>Accuracy of the response</t>
+    <t>Accuracy of the participant's response</t>
   </si>
   <si>
     <t>0;1</t>
@@ -159,19 +183,33 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="等线"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -179,37 +217,38 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="等线"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="等线 Light"/>
+      <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="major"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -217,7 +256,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -225,82 +264,89 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -504,6 +550,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -525,7 +586,7 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thick">
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -534,17 +595,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thick">
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.399975585192419"/>
       </bottom>
       <diagonal/>
     </border>
@@ -615,31 +667,20 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -648,124 +689,134 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -819,7 +870,7 @@
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -829,7 +880,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -839,44 +890,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -903,15 +954,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -938,7 +988,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -950,131 +999,160 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1086,31 +1164,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
-    <col min="2" max="2" width="42.25" customWidth="1"/>
-    <col min="3" max="3" width="23.3333333333333" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
+    <col min="1" max="1" width="30.9090909090909" customWidth="1"/>
+    <col min="2" max="2" width="98.3636363636364" customWidth="1"/>
+    <col min="3" max="3" width="26.3636363636364" customWidth="1"/>
+    <col min="4" max="4" width="21.3636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1139,152 +1217,221 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
         <v>37</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B15" t="s">
         <v>39</v>
       </c>
-      <c r="D13" t="s">
-        <v>10</v>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>